<commit_message>
Remove ac paracentesis as an exclusion
</commit_message>
<xml_diff>
--- a/codes/progression_surgery_codes_exclusions.xlsx
+++ b/codes/progression_surgery_codes_exclusions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/resmed202100066-Glaucoma_PRS/andrewholmes2024/summer2025/outcomes/codes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D25B12-805C-ED4C-AAE2-322A3FF4F691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEB147F-6A9C-7942-AD47-FE8F0CACD365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4660" yWindow="-21100" windowWidth="25600" windowHeight="21100" activeTab="3" xr2:uid="{50CFBF05-B7E9-BF4A-8961-70BF8FF71AD6}"/>
+    <workbookView xWindow="-4660" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{50CFBF05-B7E9-BF4A-8961-70BF8FF71AD6}"/>
   </bookViews>
   <sheets>
     <sheet name="self_report" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="308">
   <si>
     <t>Corneoscleral trephine</t>
   </si>
@@ -459,12 +459,6 @@
     <t>C67.9 Unspecified other operations on ciliary body</t>
   </si>
   <si>
-    <t>C692</t>
-  </si>
-  <si>
-    <t>C69.2 Paracentesis of anterior chamber of eye</t>
-  </si>
-  <si>
     <t>150 Irodotomy</t>
   </si>
   <si>
@@ -483,9 +477,6 @@
     <t>156 Cyclodialysis</t>
   </si>
   <si>
-    <t>158.1 Other operations on anterior chamber : paracentesis</t>
-  </si>
-  <si>
     <t>7256.</t>
   </si>
   <si>
@@ -510,9 +501,6 @@
     <t>1573</t>
   </si>
   <si>
-    <t>1581</t>
-  </si>
-  <si>
     <t>1574</t>
   </si>
   <si>
@@ -945,12 +933,6 @@
     <t>XE0BO</t>
   </si>
   <si>
-    <t>72621</t>
-  </si>
-  <si>
-    <t>Paracentesis of anterior chamber</t>
-  </si>
-  <si>
     <t xml:space="preserve">Creation of guarded fistula to sclera (OPCS4 C601) </t>
   </si>
   <si>
@@ -982,9 +964,6 @@
   </si>
   <si>
     <t>Laser photocoagulation of ciliary body (C664)</t>
-  </si>
-  <si>
-    <t>Paracentesis of anterior chamber of eye (C692)</t>
   </si>
 </sst>
 </file>
@@ -1527,8 +1506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60CF15B7-22DE-5845-80EA-57A73503675F}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView zoomScale="156" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A7" zoomScale="156" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1771,67 +1750,63 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>139</v>
+        <v>63</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>140</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1843,7 +1818,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView zoomScale="110" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1861,55 +1836,55 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>67</v>
@@ -1917,35 +1892,31 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>147</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>69</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>160</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1956,8 +1927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209AAC4B-633B-8D4C-8F7E-1A9573C5BFCB}">
   <dimension ref="A1:C113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="127" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="127" workbookViewId="0">
+      <selection activeCell="B139" sqref="B139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1977,645 +1948,645 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C25" s="2"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C29" s="2"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C30" s="2"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C32" s="2"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C33" s="2"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C34" s="2"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C35" s="2"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C36" s="2"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C37" s="2"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C38" s="2"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C39" s="2"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C40" s="2"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C41" s="2"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C42" s="2"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C43" s="2"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C44" s="2"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C45" s="2"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C46" s="2"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C47" s="2"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>301</v>
+        <v>42</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>302</v>
+        <v>43</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>43</v>
@@ -2623,15 +2594,15 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>45</v>
@@ -2639,23 +2610,23 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>41</v>
@@ -2663,175 +2634,175 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>46</v>
+        <v>157</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>162</v>
+        <v>78</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>78</v>
+        <v>18</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>79</v>
+        <v>19</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>22</v>
+        <v>159</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>23</v>
+        <v>297</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>163</v>
+        <v>15</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>304</v>
+        <v>17</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>32</v>
+        <v>160</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>164</v>
+        <v>80</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>80</v>
+        <v>161</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>81</v>
+        <v>26</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>165</v>
+        <v>28</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>75</v>
+        <v>162</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>25</v>
@@ -2839,7 +2810,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>167</v>
+        <v>75</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>25</v>
@@ -2847,26 +2818,26 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>75</v>
+        <v>12</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
@@ -2874,48 +2845,43 @@
         <v>73</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>8</v>
+        <v>145</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A113" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B113" s="1" t="s">
         <v>7</v>
       </c>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B113" s="1"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B52">
@@ -2929,8 +2895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2066806-BCE0-B748-9DDB-90B46CB7534A}">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView zoomScale="118" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView topLeftCell="A35" zoomScale="118" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2948,430 +2914,425 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="B26" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B27" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B28" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B29" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B30" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B31" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B32" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B33" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B34" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B35" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B36" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B37" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B38" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B39" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="B40" t="s">
-        <v>314</v>
+        <v>287</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>290</v>
+        <v>47</v>
       </c>
       <c r="B41" t="s">
-        <v>291</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>48</v>
+        <v>157</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B44" t="s">
-        <v>0</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B45" t="s">
-        <v>79</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B46" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B47" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B48" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
       <c r="B49" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>148</v>
+        <v>8</v>
       </c>
       <c r="B50" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B51" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>10</v>
+        <v>145</v>
       </c>
       <c r="B52" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B53" t="s">
-        <v>7</v>
-      </c>
+      <c r="A53" s="1"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B21">

</xml_diff>